<commit_message>
COMMIT for copy file tool
</commit_message>
<xml_diff>
--- a/src/rechard/dbs/tool/translation/R12_Translationsv1.1.xlsx
+++ b/src/rechard/dbs/tool/translation/R12_Translationsv1.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8370" tabRatio="582" activeTab="1"/>
+    <workbookView windowWidth="20385" windowHeight="8370" tabRatio="582"/>
   </bookViews>
   <sheets>
     <sheet name="config properties" sheetId="1" r:id="rId1"/>
@@ -189,94 +189,94 @@
     <t>請選擇細分類</t>
   </si>
   <si>
-    <t>D:\code\DBS_CB\CORP_PSO_SRC\corpbanking-config\web-resources\com\s1\payments\trnint\Resources_pso.properties</t>
-  </si>
-  <si>
-    <t>reasonForPayment.text.1</t>
+    <t>D:\code\DBS_CB\CORP_PSO_SRC\corpbanking-config\web-resources\com\s1\banking\efd\upload\user\EFD-Resources_pso.properties</t>
+  </si>
+  <si>
+    <t>reasonForPayment.274.text.1</t>
   </si>
   <si>
     <t>運輸支出</t>
   </si>
   <si>
-    <t>reasonForPayment.text.2</t>
+    <t>reasonForPayment.274.text.2</t>
   </si>
   <si>
     <t>保險支出</t>
   </si>
   <si>
-    <t>reasonForPayment.text.3</t>
+    <t>reasonForPayment.274.text.3</t>
   </si>
   <si>
     <t>旅行支出</t>
   </si>
   <si>
-    <t>reasonForPayment.text.4</t>
+    <t>reasonForPayment.274.text.4</t>
   </si>
   <si>
     <t>運保費及旅行以外之其他服務支出</t>
   </si>
   <si>
-    <t>reasonForPayment.text.5</t>
+    <t>reasonForPayment.274.text.5</t>
   </si>
   <si>
     <t>本國資金流出</t>
   </si>
   <si>
-    <t>reasonForPayment.text.6</t>
+    <t>reasonForPayment.274.text.6</t>
   </si>
   <si>
     <t>外國資金流出</t>
   </si>
   <si>
-    <t>reasonForPayment.text.7</t>
+    <t>reasonForPayment.274.text.7</t>
   </si>
   <si>
     <t>薪資支出</t>
   </si>
   <si>
-    <t>reasonForPayment.text.8</t>
+    <t>reasonForPayment.274.text.8</t>
   </si>
   <si>
     <t>外資投資所得(不含資本利得或損失)</t>
   </si>
   <si>
-    <t>reasonForPayment.text.9</t>
+    <t>reasonForPayment.274.text.9</t>
   </si>
   <si>
     <t>移轉支出</t>
   </si>
   <si>
-    <t>reasonForPayment.text.10</t>
+    <t>reasonForPayment.274.text.10</t>
   </si>
   <si>
     <t>其他國外交易</t>
   </si>
   <si>
-    <t>reasonForPayment.text.11</t>
+    <t>reasonForPayment.274.text.11</t>
   </si>
   <si>
     <t>國內交易</t>
   </si>
   <si>
-    <t>reasonForPayment.text.12</t>
+    <t>reasonForPayment.274.text.12</t>
   </si>
   <si>
     <t>進口通關的貨款</t>
   </si>
   <si>
-    <t>reasonForPayment.text.13</t>
+    <t>reasonForPayment.274.text.13</t>
   </si>
   <si>
     <t>未經我國進口通關的國外貨款支出</t>
   </si>
   <si>
-    <t>reasonForPayment.text.14</t>
+    <t>reasonForPayment.274.text.14</t>
   </si>
   <si>
     <t>支付國外但供貨來自境內之貨款</t>
   </si>
   <si>
-    <t>reasonForPayment.text.15</t>
+    <t>reasonForPayment.274.text.15</t>
   </si>
   <si>
     <t>其他貨款</t>
@@ -312,11 +312,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -364,13 +364,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
@@ -383,7 +376,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -404,8 +405,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -419,7 +421,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -427,7 +429,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -441,10 +443,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -465,7 +468,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -490,30 +507,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -552,7 +545,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -564,91 +581,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -660,55 +599,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -721,6 +612,108 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -762,15 +755,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -786,17 +770,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -825,6 +803,41 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -839,36 +852,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -877,16 +870,16 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -895,119 +888,119 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="28" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1049,19 +1042,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1073,7 +1063,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1399,13 +1389,13 @@
   <sheetPr/>
   <dimension ref="A1:G232"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="53.3833333333333" style="1" customWidth="1"/>
+    <col min="1" max="1" width="157.125" style="1" customWidth="1"/>
     <col min="2" max="2" width="34.625" style="1" customWidth="1"/>
     <col min="3" max="3" width="44.875" style="2" customWidth="1"/>
     <col min="4" max="4" width="18.125" style="3" customWidth="1"/>
@@ -1658,7 +1648,7 @@
       <c r="D13" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="15" t="s">
         <v>51</v>
       </c>
       <c r="F13" s="13" t="s">
@@ -1675,7 +1665,7 @@
       <c r="D14" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="15" t="s">
         <v>55</v>
       </c>
       <c r="F14" s="13" t="s">
@@ -1692,10 +1682,10 @@
       <c r="B15" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="23" t="s">
+      <c r="C15" s="16"/>
+      <c r="D15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="22" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1706,10 +1696,10 @@
       <c r="B16" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="24" t="s">
+      <c r="C16" s="16"/>
+      <c r="D16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="23" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1720,10 +1710,10 @@
       <c r="B17" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="24" t="s">
+      <c r="C17" s="16"/>
+      <c r="D17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="23" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1734,10 +1724,10 @@
       <c r="B18" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="17"/>
-      <c r="D18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="24" t="s">
+      <c r="C18" s="16"/>
+      <c r="D18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="23" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1748,10 +1738,10 @@
       <c r="B19" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="24" t="s">
+      <c r="C19" s="16"/>
+      <c r="D19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="23" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1762,10 +1752,10 @@
       <c r="B20" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="24" t="s">
+      <c r="C20" s="16"/>
+      <c r="D20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="23" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1776,10 +1766,10 @@
       <c r="B21" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="24" t="s">
+      <c r="C21" s="16"/>
+      <c r="D21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="23" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1790,10 +1780,10 @@
       <c r="B22" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C22" s="17"/>
-      <c r="D22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="24" t="s">
+      <c r="C22" s="16"/>
+      <c r="D22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="23" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1804,10 +1794,10 @@
       <c r="B23" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="24" t="s">
+      <c r="C23" s="16"/>
+      <c r="D23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="23" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1818,10 +1808,10 @@
       <c r="B24" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="24" t="s">
+      <c r="C24" s="16"/>
+      <c r="D24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="23" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1832,10 +1822,10 @@
       <c r="B25" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C25" s="17"/>
-      <c r="D25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="24" t="s">
+      <c r="C25" s="16"/>
+      <c r="D25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="23" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1846,10 +1836,10 @@
       <c r="B26" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C26" s="17"/>
+      <c r="C26" s="16"/>
       <c r="D26" s="3"/>
       <c r="F26" s="3"/>
-      <c r="G26" s="25" t="s">
+      <c r="G26" s="24" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1860,10 +1850,10 @@
       <c r="B27" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C27" s="17"/>
+      <c r="C27" s="16"/>
       <c r="D27" s="3"/>
       <c r="F27" s="3"/>
-      <c r="G27" s="25" t="s">
+      <c r="G27" s="24" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1874,10 +1864,10 @@
       <c r="B28" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C28" s="17"/>
+      <c r="C28" s="16"/>
       <c r="D28" s="3"/>
       <c r="F28" s="3"/>
-      <c r="G28" s="25" t="s">
+      <c r="G28" s="24" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1888,498 +1878,501 @@
       <c r="B29" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C29" s="17"/>
+      <c r="C29" s="16"/>
       <c r="D29" s="3"/>
       <c r="F29" s="3"/>
-      <c r="G29" s="25" t="s">
+      <c r="G29" s="24" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="30" s="1" customFormat="1" spans="3:7">
-      <c r="C30" s="17"/>
+    <row r="30" s="1" customFormat="1" spans="1:7">
+      <c r="A30" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="16"/>
       <c r="D30" s="3"/>
       <c r="E30" s="4"/>
       <c r="F30" s="3"/>
       <c r="G30" s="5"/>
     </row>
     <row r="31" s="1" customFormat="1" spans="3:7">
-      <c r="C31" s="17"/>
+      <c r="C31" s="16"/>
       <c r="D31" s="3"/>
       <c r="E31" s="4"/>
       <c r="F31" s="3"/>
       <c r="G31" s="5"/>
     </row>
     <row r="32" s="1" customFormat="1" spans="3:7">
-      <c r="C32" s="17"/>
+      <c r="C32" s="16"/>
       <c r="D32" s="3"/>
       <c r="E32" s="4"/>
       <c r="F32" s="3"/>
       <c r="G32" s="5"/>
     </row>
     <row r="33" s="1" customFormat="1" spans="3:7">
-      <c r="C33" s="17"/>
+      <c r="C33" s="16"/>
       <c r="D33" s="3"/>
       <c r="E33" s="4"/>
       <c r="F33" s="3"/>
       <c r="G33" s="5"/>
     </row>
     <row r="34" s="1" customFormat="1" spans="3:7">
-      <c r="C34" s="17"/>
+      <c r="C34" s="16"/>
       <c r="D34" s="3"/>
       <c r="E34" s="4"/>
       <c r="F34" s="3"/>
       <c r="G34" s="5"/>
     </row>
     <row r="35" s="1" customFormat="1" spans="3:7">
-      <c r="C35" s="17"/>
+      <c r="C35" s="16"/>
       <c r="D35" s="3"/>
       <c r="E35" s="4"/>
       <c r="F35" s="3"/>
       <c r="G35" s="5"/>
     </row>
     <row r="36" s="1" customFormat="1" spans="3:7">
-      <c r="C36" s="17"/>
+      <c r="C36" s="16"/>
       <c r="D36" s="3"/>
       <c r="E36" s="4"/>
       <c r="F36" s="3"/>
       <c r="G36" s="5"/>
     </row>
     <row r="37" s="1" customFormat="1" spans="3:7">
-      <c r="C37" s="17"/>
+      <c r="C37" s="16"/>
       <c r="D37" s="3"/>
       <c r="E37" s="4"/>
       <c r="F37" s="3"/>
       <c r="G37" s="5"/>
     </row>
     <row r="38" s="1" customFormat="1" spans="3:7">
-      <c r="C38" s="17"/>
+      <c r="C38" s="16"/>
       <c r="D38" s="3"/>
       <c r="E38" s="4"/>
       <c r="F38" s="3"/>
       <c r="G38" s="5"/>
     </row>
     <row r="39" s="1" customFormat="1" spans="3:7">
-      <c r="C39" s="17"/>
+      <c r="C39" s="16"/>
       <c r="D39" s="3"/>
       <c r="E39" s="4"/>
       <c r="F39" s="3"/>
       <c r="G39" s="5"/>
     </row>
     <row r="40" s="1" customFormat="1" spans="3:7">
-      <c r="C40" s="17"/>
+      <c r="C40" s="16"/>
       <c r="D40" s="3"/>
       <c r="E40" s="4"/>
       <c r="F40" s="3"/>
       <c r="G40" s="5"/>
     </row>
     <row r="41" s="1" customFormat="1" spans="3:7">
-      <c r="C41" s="17"/>
+      <c r="C41" s="16"/>
       <c r="D41" s="3"/>
       <c r="E41" s="4"/>
       <c r="F41" s="3"/>
       <c r="G41" s="5"/>
     </row>
     <row r="42" s="1" customFormat="1" spans="3:7">
-      <c r="C42" s="17"/>
+      <c r="C42" s="16"/>
       <c r="D42" s="3"/>
       <c r="E42" s="4"/>
       <c r="F42" s="3"/>
       <c r="G42" s="5"/>
     </row>
     <row r="43" s="1" customFormat="1" spans="3:7">
-      <c r="C43" s="17"/>
+      <c r="C43" s="16"/>
       <c r="D43" s="3"/>
       <c r="E43" s="4"/>
       <c r="F43" s="3"/>
       <c r="G43" s="5"/>
     </row>
     <row r="44" s="1" customFormat="1" spans="3:7">
-      <c r="C44" s="17"/>
+      <c r="C44" s="16"/>
       <c r="D44" s="3"/>
       <c r="E44" s="4"/>
       <c r="F44" s="3"/>
       <c r="G44" s="5"/>
     </row>
     <row r="45" s="1" customFormat="1" spans="3:7">
-      <c r="C45" s="17"/>
+      <c r="C45" s="16"/>
       <c r="D45" s="3"/>
       <c r="E45" s="4"/>
       <c r="F45" s="3"/>
       <c r="G45" s="5"/>
     </row>
     <row r="46" s="1" customFormat="1" spans="3:7">
-      <c r="C46" s="17"/>
+      <c r="C46" s="16"/>
       <c r="D46" s="3"/>
       <c r="E46" s="4"/>
       <c r="F46" s="3"/>
       <c r="G46" s="5"/>
     </row>
     <row r="47" s="1" customFormat="1" spans="3:7">
-      <c r="C47" s="17"/>
+      <c r="C47" s="16"/>
       <c r="D47" s="3"/>
       <c r="E47" s="4"/>
       <c r="F47" s="3"/>
       <c r="G47" s="5"/>
     </row>
     <row r="48" s="1" customFormat="1" spans="3:7">
-      <c r="C48" s="17"/>
+      <c r="C48" s="16"/>
       <c r="D48" s="3"/>
       <c r="E48" s="4"/>
       <c r="F48" s="3"/>
       <c r="G48" s="5"/>
     </row>
     <row r="49" s="1" customFormat="1" spans="3:7">
-      <c r="C49" s="17"/>
+      <c r="C49" s="16"/>
       <c r="D49" s="3"/>
       <c r="E49" s="4"/>
       <c r="F49" s="3"/>
       <c r="G49" s="5"/>
     </row>
     <row r="50" s="1" customFormat="1" spans="3:7">
-      <c r="C50" s="17"/>
+      <c r="C50" s="16"/>
       <c r="D50" s="3"/>
       <c r="E50" s="4"/>
       <c r="F50" s="3"/>
       <c r="G50" s="5"/>
     </row>
     <row r="51" s="1" customFormat="1" spans="3:7">
-      <c r="C51" s="17"/>
+      <c r="C51" s="16"/>
       <c r="D51" s="3"/>
       <c r="E51" s="4"/>
       <c r="F51" s="3"/>
       <c r="G51" s="5"/>
     </row>
     <row r="52" s="1" customFormat="1" spans="3:7">
-      <c r="C52" s="17"/>
+      <c r="C52" s="16"/>
       <c r="D52" s="3"/>
       <c r="E52" s="4"/>
       <c r="F52" s="3"/>
       <c r="G52" s="5"/>
     </row>
     <row r="53" s="1" customFormat="1" spans="3:7">
-      <c r="C53" s="17"/>
+      <c r="C53" s="16"/>
       <c r="D53" s="3"/>
       <c r="E53" s="4"/>
       <c r="F53" s="3"/>
       <c r="G53" s="5"/>
     </row>
     <row r="54" s="1" customFormat="1" spans="3:7">
-      <c r="C54" s="17"/>
+      <c r="C54" s="16"/>
       <c r="D54" s="3"/>
       <c r="E54" s="4"/>
       <c r="F54" s="3"/>
       <c r="G54" s="5"/>
     </row>
     <row r="55" s="1" customFormat="1" spans="3:7">
-      <c r="C55" s="17"/>
+      <c r="C55" s="16"/>
       <c r="D55" s="3"/>
       <c r="E55" s="4"/>
       <c r="F55" s="3"/>
       <c r="G55" s="5"/>
     </row>
     <row r="56" s="1" customFormat="1" spans="3:7">
-      <c r="C56" s="17"/>
+      <c r="C56" s="16"/>
       <c r="D56" s="3"/>
       <c r="E56" s="4"/>
       <c r="F56" s="3"/>
       <c r="G56" s="5"/>
     </row>
     <row r="57" s="1" customFormat="1" spans="3:7">
-      <c r="C57" s="17"/>
+      <c r="C57" s="16"/>
       <c r="D57" s="3"/>
       <c r="E57" s="4"/>
       <c r="F57" s="3"/>
       <c r="G57" s="5"/>
     </row>
     <row r="58" s="1" customFormat="1" spans="3:7">
-      <c r="C58" s="17"/>
+      <c r="C58" s="16"/>
       <c r="D58" s="3"/>
       <c r="E58" s="4"/>
       <c r="F58" s="3"/>
       <c r="G58" s="5"/>
     </row>
     <row r="59" s="1" customFormat="1" spans="3:7">
-      <c r="C59" s="17"/>
+      <c r="C59" s="16"/>
       <c r="D59" s="3"/>
       <c r="E59" s="4"/>
       <c r="F59" s="3"/>
       <c r="G59" s="5"/>
     </row>
     <row r="60" s="1" customFormat="1" spans="3:7">
-      <c r="C60" s="17"/>
+      <c r="C60" s="16"/>
       <c r="D60" s="3"/>
       <c r="E60" s="4"/>
       <c r="F60" s="3"/>
       <c r="G60" s="5"/>
     </row>
     <row r="61" s="1" customFormat="1" spans="3:7">
-      <c r="C61" s="17"/>
+      <c r="C61" s="16"/>
       <c r="D61" s="3"/>
       <c r="E61" s="4"/>
       <c r="F61" s="3"/>
       <c r="G61" s="5"/>
     </row>
     <row r="62" s="1" customFormat="1" spans="3:7">
-      <c r="C62" s="17"/>
+      <c r="C62" s="16"/>
       <c r="D62" s="3"/>
       <c r="E62" s="4"/>
       <c r="F62" s="3"/>
       <c r="G62" s="5"/>
     </row>
     <row r="63" s="1" customFormat="1" spans="3:7">
-      <c r="C63" s="17"/>
+      <c r="C63" s="16"/>
       <c r="D63" s="3"/>
       <c r="E63" s="4"/>
       <c r="F63" s="3"/>
       <c r="G63" s="5"/>
     </row>
     <row r="64" s="1" customFormat="1" spans="3:7">
-      <c r="C64" s="17"/>
+      <c r="C64" s="16"/>
       <c r="D64" s="3"/>
       <c r="E64" s="4"/>
       <c r="F64" s="3"/>
       <c r="G64" s="5"/>
     </row>
     <row r="65" s="1" customFormat="1" spans="3:7">
-      <c r="C65" s="17"/>
+      <c r="C65" s="16"/>
       <c r="D65" s="3"/>
       <c r="E65" s="4"/>
       <c r="F65" s="3"/>
       <c r="G65" s="5"/>
     </row>
     <row r="66" s="1" customFormat="1" spans="3:7">
-      <c r="C66" s="17"/>
+      <c r="C66" s="16"/>
       <c r="D66" s="3"/>
       <c r="E66" s="4"/>
       <c r="F66" s="3"/>
       <c r="G66" s="5"/>
     </row>
     <row r="67" s="1" customFormat="1" spans="3:7">
-      <c r="C67" s="17"/>
+      <c r="C67" s="16"/>
       <c r="D67" s="3"/>
       <c r="E67" s="4"/>
       <c r="F67" s="3"/>
       <c r="G67" s="5"/>
     </row>
     <row r="68" s="1" customFormat="1" spans="3:7">
-      <c r="C68" s="17"/>
+      <c r="C68" s="16"/>
       <c r="D68" s="3"/>
       <c r="E68" s="4"/>
       <c r="F68" s="3"/>
       <c r="G68" s="5"/>
     </row>
     <row r="69" s="1" customFormat="1" spans="3:7">
-      <c r="C69" s="17"/>
+      <c r="C69" s="16"/>
       <c r="D69" s="3"/>
       <c r="E69" s="4"/>
       <c r="F69" s="3"/>
       <c r="G69" s="5"/>
     </row>
     <row r="70" s="1" customFormat="1" spans="3:7">
-      <c r="C70" s="17"/>
+      <c r="C70" s="16"/>
       <c r="D70" s="3"/>
       <c r="E70" s="4"/>
       <c r="F70" s="3"/>
       <c r="G70" s="5"/>
     </row>
     <row r="71" s="1" customFormat="1" spans="3:7">
-      <c r="C71" s="17"/>
+      <c r="C71" s="16"/>
       <c r="D71" s="3"/>
       <c r="E71" s="4"/>
       <c r="F71" s="3"/>
       <c r="G71" s="5"/>
     </row>
     <row r="72" s="1" customFormat="1" spans="3:7">
-      <c r="C72" s="17"/>
+      <c r="C72" s="16"/>
       <c r="D72" s="3"/>
       <c r="E72" s="4"/>
       <c r="F72" s="3"/>
       <c r="G72" s="5"/>
     </row>
     <row r="73" s="1" customFormat="1" spans="3:7">
-      <c r="C73" s="17"/>
+      <c r="C73" s="16"/>
       <c r="D73" s="3"/>
       <c r="E73" s="4"/>
       <c r="F73" s="3"/>
       <c r="G73" s="5"/>
     </row>
     <row r="74" s="1" customFormat="1" spans="3:7">
-      <c r="C74" s="17"/>
+      <c r="C74" s="16"/>
       <c r="D74" s="3"/>
       <c r="E74" s="4"/>
       <c r="F74" s="3"/>
       <c r="G74" s="5"/>
     </row>
     <row r="75" s="1" customFormat="1" spans="3:7">
-      <c r="C75" s="17"/>
+      <c r="C75" s="16"/>
       <c r="D75" s="3"/>
       <c r="E75" s="4"/>
       <c r="F75" s="3"/>
       <c r="G75" s="5"/>
     </row>
     <row r="76" s="1" customFormat="1" spans="3:7">
-      <c r="C76" s="17"/>
+      <c r="C76" s="16"/>
       <c r="D76" s="3"/>
       <c r="E76" s="4"/>
       <c r="F76" s="3"/>
       <c r="G76" s="5"/>
     </row>
     <row r="77" s="1" customFormat="1" spans="3:7">
-      <c r="C77" s="17"/>
+      <c r="C77" s="16"/>
       <c r="D77" s="3"/>
       <c r="E77" s="4"/>
       <c r="F77" s="3"/>
       <c r="G77" s="5"/>
     </row>
     <row r="78" s="1" customFormat="1" spans="3:7">
-      <c r="C78" s="17"/>
+      <c r="C78" s="16"/>
       <c r="D78" s="3"/>
       <c r="E78" s="4"/>
       <c r="F78" s="3"/>
       <c r="G78" s="5"/>
     </row>
     <row r="79" s="1" customFormat="1" spans="3:7">
-      <c r="C79" s="17"/>
+      <c r="C79" s="16"/>
       <c r="D79" s="3"/>
       <c r="E79" s="4"/>
       <c r="F79" s="3"/>
       <c r="G79" s="5"/>
     </row>
     <row r="80" s="1" customFormat="1" spans="3:7">
-      <c r="C80" s="17"/>
+      <c r="C80" s="16"/>
       <c r="D80" s="3"/>
       <c r="E80" s="4"/>
       <c r="F80" s="3"/>
       <c r="G80" s="5"/>
     </row>
     <row r="81" s="1" customFormat="1" spans="3:7">
-      <c r="C81" s="17"/>
+      <c r="C81" s="16"/>
       <c r="D81" s="3"/>
       <c r="E81" s="4"/>
       <c r="F81" s="3"/>
       <c r="G81" s="5"/>
     </row>
     <row r="82" s="1" customFormat="1" spans="3:7">
-      <c r="C82" s="17"/>
+      <c r="C82" s="16"/>
       <c r="D82" s="3"/>
       <c r="E82" s="4"/>
       <c r="F82" s="3"/>
       <c r="G82" s="5"/>
     </row>
     <row r="83" s="1" customFormat="1" spans="3:7">
-      <c r="C83" s="17"/>
+      <c r="C83" s="16"/>
       <c r="D83" s="3"/>
       <c r="E83" s="4"/>
       <c r="F83" s="3"/>
       <c r="G83" s="5"/>
     </row>
     <row r="84" s="1" customFormat="1" spans="3:7">
-      <c r="C84" s="17"/>
+      <c r="C84" s="16"/>
       <c r="D84" s="3"/>
       <c r="E84" s="4"/>
       <c r="F84" s="3"/>
       <c r="G84" s="5"/>
     </row>
     <row r="85" s="1" customFormat="1" spans="3:7">
-      <c r="C85" s="17"/>
+      <c r="C85" s="16"/>
       <c r="D85" s="3"/>
       <c r="E85" s="4"/>
       <c r="F85" s="3"/>
       <c r="G85" s="5"/>
     </row>
     <row r="86" s="1" customFormat="1" spans="3:7">
-      <c r="C86" s="17"/>
+      <c r="C86" s="16"/>
       <c r="D86" s="3"/>
       <c r="E86" s="4"/>
       <c r="F86" s="3"/>
       <c r="G86" s="5"/>
     </row>
     <row r="87" s="1" customFormat="1" spans="3:7">
-      <c r="C87" s="17"/>
+      <c r="C87" s="16"/>
       <c r="D87" s="3"/>
       <c r="E87" s="4"/>
       <c r="F87" s="3"/>
       <c r="G87" s="5"/>
     </row>
     <row r="88" s="1" customFormat="1" spans="3:7">
-      <c r="C88" s="17"/>
+      <c r="C88" s="16"/>
       <c r="D88" s="3"/>
       <c r="E88" s="4"/>
       <c r="F88" s="3"/>
       <c r="G88" s="5"/>
     </row>
     <row r="89" s="1" customFormat="1" spans="3:7">
-      <c r="C89" s="17"/>
+      <c r="C89" s="16"/>
       <c r="D89" s="3"/>
       <c r="E89" s="4"/>
       <c r="F89" s="3"/>
       <c r="G89" s="5"/>
     </row>
     <row r="90" s="1" customFormat="1" spans="3:7">
-      <c r="C90" s="17"/>
+      <c r="C90" s="16"/>
       <c r="D90" s="3"/>
       <c r="E90" s="4"/>
       <c r="F90" s="3"/>
       <c r="G90" s="5"/>
     </row>
     <row r="91" s="1" customFormat="1" spans="3:7">
-      <c r="C91" s="17"/>
+      <c r="C91" s="16"/>
       <c r="D91" s="3"/>
       <c r="E91" s="4"/>
       <c r="F91" s="3"/>
       <c r="G91" s="5"/>
     </row>
     <row r="92" s="1" customFormat="1" spans="3:7">
-      <c r="C92" s="17"/>
+      <c r="C92" s="16"/>
       <c r="D92" s="3"/>
       <c r="E92" s="4"/>
       <c r="F92" s="3"/>
       <c r="G92" s="5"/>
     </row>
     <row r="93" s="1" customFormat="1" spans="3:7">
-      <c r="C93" s="17"/>
+      <c r="C93" s="16"/>
       <c r="D93" s="3"/>
       <c r="E93" s="4"/>
       <c r="F93" s="3"/>
       <c r="G93" s="5"/>
     </row>
     <row r="94" s="1" customFormat="1" spans="3:7">
-      <c r="C94" s="17"/>
+      <c r="C94" s="16"/>
       <c r="D94" s="3"/>
       <c r="E94" s="4"/>
       <c r="F94" s="3"/>
       <c r="G94" s="5"/>
     </row>
     <row r="95" s="1" customFormat="1" spans="3:7">
-      <c r="C95" s="17"/>
+      <c r="C95" s="16"/>
       <c r="D95" s="3"/>
       <c r="E95" s="4"/>
       <c r="F95" s="3"/>
       <c r="G95" s="5"/>
     </row>
     <row r="96" s="1" customFormat="1" spans="3:7">
-      <c r="C96" s="17"/>
+      <c r="C96" s="16"/>
       <c r="D96" s="3"/>
       <c r="E96" s="4"/>
       <c r="F96" s="3"/>
       <c r="G96" s="5"/>
     </row>
     <row r="97" s="1" customFormat="1" spans="3:7">
-      <c r="C97" s="17"/>
+      <c r="C97" s="16"/>
       <c r="D97" s="3"/>
       <c r="E97" s="4"/>
       <c r="F97" s="3"/>
       <c r="G97" s="5"/>
     </row>
     <row r="98" s="1" customFormat="1" spans="3:7">
-      <c r="C98" s="17"/>
+      <c r="C98" s="16"/>
       <c r="D98" s="3"/>
       <c r="E98" s="4"/>
       <c r="F98" s="3"/>
       <c r="G98" s="5"/>
     </row>
     <row r="99" s="1" customFormat="1" spans="3:7">
-      <c r="C99" s="17"/>
+      <c r="C99" s="16"/>
       <c r="D99" s="3"/>
       <c r="E99" s="4"/>
       <c r="F99" s="3"/>
@@ -3328,7 +3321,7 @@
   <sheetPr/>
   <dimension ref="A1:G232"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -3525,7 +3518,7 @@
       </c>
     </row>
     <row r="10" s="1" customFormat="1" ht="15.75" customHeight="1" spans="1:7">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -3606,7 +3599,7 @@
       <c r="D13" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="15" t="s">
         <v>51</v>
       </c>
       <c r="F13" s="13" t="s">
@@ -3623,7 +3616,7 @@
       <c r="D14" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="15" t="s">
         <v>55</v>
       </c>
       <c r="F14" s="13" t="s">
@@ -3634,595 +3627,595 @@
       </c>
     </row>
     <row r="15" s="1" customFormat="1" spans="3:7">
-      <c r="C15" s="17"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
     </row>
     <row r="16" s="1" customFormat="1" spans="3:7">
-      <c r="C16" s="17"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="21"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="20"/>
     </row>
     <row r="17" s="1" customFormat="1" spans="3:7">
-      <c r="C17" s="17"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="21"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="20"/>
     </row>
     <row r="18" s="1" customFormat="1" spans="3:7">
-      <c r="C18" s="17"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="21"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="20"/>
     </row>
     <row r="19" s="1" customFormat="1" spans="3:7">
-      <c r="C19" s="17"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="21"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="20"/>
     </row>
     <row r="20" s="1" customFormat="1" spans="3:7">
-      <c r="C20" s="17"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="21"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="20"/>
     </row>
     <row r="21" s="1" customFormat="1" spans="3:7">
-      <c r="C21" s="17"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="21"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="20"/>
     </row>
     <row r="22" s="1" customFormat="1" spans="3:7">
-      <c r="C22" s="17"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="22"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="21"/>
     </row>
     <row r="23" s="1" customFormat="1" spans="3:7">
-      <c r="C23" s="17"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="22"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="21"/>
     </row>
     <row r="24" s="1" customFormat="1" spans="3:7">
-      <c r="C24" s="17"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="22"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="21"/>
     </row>
     <row r="25" s="1" customFormat="1" spans="3:7">
-      <c r="C25" s="17"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="22"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="21"/>
     </row>
     <row r="26" s="1" customFormat="1" spans="3:7">
-      <c r="C26" s="17"/>
+      <c r="C26" s="16"/>
       <c r="D26" s="3"/>
       <c r="E26" s="4"/>
       <c r="F26" s="3"/>
       <c r="G26" s="5"/>
     </row>
     <row r="27" s="1" customFormat="1" spans="3:7">
-      <c r="C27" s="17"/>
+      <c r="C27" s="16"/>
       <c r="D27" s="3"/>
       <c r="E27" s="4"/>
       <c r="F27" s="3"/>
       <c r="G27" s="5"/>
     </row>
     <row r="28" s="1" customFormat="1" spans="3:7">
-      <c r="C28" s="17"/>
+      <c r="C28" s="16"/>
       <c r="D28" s="3"/>
       <c r="E28" s="4"/>
       <c r="F28" s="3"/>
       <c r="G28" s="5"/>
     </row>
     <row r="29" s="1" customFormat="1" spans="3:7">
-      <c r="C29" s="17"/>
+      <c r="C29" s="16"/>
       <c r="D29" s="3"/>
       <c r="E29" s="4"/>
       <c r="F29" s="3"/>
       <c r="G29" s="5"/>
     </row>
     <row r="30" s="1" customFormat="1" spans="3:7">
-      <c r="C30" s="17"/>
+      <c r="C30" s="16"/>
       <c r="D30" s="3"/>
       <c r="E30" s="4"/>
       <c r="F30" s="3"/>
       <c r="G30" s="5"/>
     </row>
     <row r="31" s="1" customFormat="1" spans="3:7">
-      <c r="C31" s="17"/>
+      <c r="C31" s="16"/>
       <c r="D31" s="3"/>
       <c r="E31" s="4"/>
       <c r="F31" s="3"/>
       <c r="G31" s="5"/>
     </row>
     <row r="32" s="1" customFormat="1" spans="3:7">
-      <c r="C32" s="17"/>
+      <c r="C32" s="16"/>
       <c r="D32" s="3"/>
       <c r="E32" s="4"/>
       <c r="F32" s="3"/>
       <c r="G32" s="5"/>
     </row>
     <row r="33" s="1" customFormat="1" spans="3:7">
-      <c r="C33" s="17"/>
+      <c r="C33" s="16"/>
       <c r="D33" s="3"/>
       <c r="E33" s="4"/>
       <c r="F33" s="3"/>
       <c r="G33" s="5"/>
     </row>
     <row r="34" s="1" customFormat="1" spans="3:7">
-      <c r="C34" s="17"/>
+      <c r="C34" s="16"/>
       <c r="D34" s="3"/>
       <c r="E34" s="4"/>
       <c r="F34" s="3"/>
       <c r="G34" s="5"/>
     </row>
     <row r="35" s="1" customFormat="1" spans="3:7">
-      <c r="C35" s="17"/>
+      <c r="C35" s="16"/>
       <c r="D35" s="3"/>
       <c r="E35" s="4"/>
       <c r="F35" s="3"/>
       <c r="G35" s="5"/>
     </row>
     <row r="36" s="1" customFormat="1" spans="3:7">
-      <c r="C36" s="17"/>
+      <c r="C36" s="16"/>
       <c r="D36" s="3"/>
       <c r="E36" s="4"/>
       <c r="F36" s="3"/>
       <c r="G36" s="5"/>
     </row>
     <row r="37" s="1" customFormat="1" spans="3:7">
-      <c r="C37" s="17"/>
+      <c r="C37" s="16"/>
       <c r="D37" s="3"/>
       <c r="E37" s="4"/>
       <c r="F37" s="3"/>
       <c r="G37" s="5"/>
     </row>
     <row r="38" s="1" customFormat="1" spans="3:7">
-      <c r="C38" s="17"/>
+      <c r="C38" s="16"/>
       <c r="D38" s="3"/>
       <c r="E38" s="4"/>
       <c r="F38" s="3"/>
       <c r="G38" s="5"/>
     </row>
     <row r="39" s="1" customFormat="1" spans="3:7">
-      <c r="C39" s="17"/>
+      <c r="C39" s="16"/>
       <c r="D39" s="3"/>
       <c r="E39" s="4"/>
       <c r="F39" s="3"/>
       <c r="G39" s="5"/>
     </row>
     <row r="40" s="1" customFormat="1" spans="3:7">
-      <c r="C40" s="17"/>
+      <c r="C40" s="16"/>
       <c r="D40" s="3"/>
       <c r="E40" s="4"/>
       <c r="F40" s="3"/>
       <c r="G40" s="5"/>
     </row>
     <row r="41" s="1" customFormat="1" spans="3:7">
-      <c r="C41" s="17"/>
+      <c r="C41" s="16"/>
       <c r="D41" s="3"/>
       <c r="E41" s="4"/>
       <c r="F41" s="3"/>
       <c r="G41" s="5"/>
     </row>
     <row r="42" s="1" customFormat="1" spans="3:7">
-      <c r="C42" s="17"/>
+      <c r="C42" s="16"/>
       <c r="D42" s="3"/>
       <c r="E42" s="4"/>
       <c r="F42" s="3"/>
       <c r="G42" s="5"/>
     </row>
     <row r="43" s="1" customFormat="1" spans="3:7">
-      <c r="C43" s="17"/>
+      <c r="C43" s="16"/>
       <c r="D43" s="3"/>
       <c r="E43" s="4"/>
       <c r="F43" s="3"/>
       <c r="G43" s="5"/>
     </row>
     <row r="44" s="1" customFormat="1" spans="3:7">
-      <c r="C44" s="17"/>
+      <c r="C44" s="16"/>
       <c r="D44" s="3"/>
       <c r="E44" s="4"/>
       <c r="F44" s="3"/>
       <c r="G44" s="5"/>
     </row>
     <row r="45" s="1" customFormat="1" spans="3:7">
-      <c r="C45" s="17"/>
+      <c r="C45" s="16"/>
       <c r="D45" s="3"/>
       <c r="E45" s="4"/>
       <c r="F45" s="3"/>
       <c r="G45" s="5"/>
     </row>
     <row r="46" s="1" customFormat="1" spans="3:7">
-      <c r="C46" s="17"/>
+      <c r="C46" s="16"/>
       <c r="D46" s="3"/>
       <c r="E46" s="4"/>
       <c r="F46" s="3"/>
       <c r="G46" s="5"/>
     </row>
     <row r="47" s="1" customFormat="1" spans="3:7">
-      <c r="C47" s="17"/>
+      <c r="C47" s="16"/>
       <c r="D47" s="3"/>
       <c r="E47" s="4"/>
       <c r="F47" s="3"/>
       <c r="G47" s="5"/>
     </row>
     <row r="48" s="1" customFormat="1" spans="3:7">
-      <c r="C48" s="17"/>
+      <c r="C48" s="16"/>
       <c r="D48" s="3"/>
       <c r="E48" s="4"/>
       <c r="F48" s="3"/>
       <c r="G48" s="5"/>
     </row>
     <row r="49" s="1" customFormat="1" spans="3:7">
-      <c r="C49" s="17"/>
+      <c r="C49" s="16"/>
       <c r="D49" s="3"/>
       <c r="E49" s="4"/>
       <c r="F49" s="3"/>
       <c r="G49" s="5"/>
     </row>
     <row r="50" s="1" customFormat="1" spans="3:7">
-      <c r="C50" s="17"/>
+      <c r="C50" s="16"/>
       <c r="D50" s="3"/>
       <c r="E50" s="4"/>
       <c r="F50" s="3"/>
       <c r="G50" s="5"/>
     </row>
     <row r="51" s="1" customFormat="1" spans="3:7">
-      <c r="C51" s="17"/>
+      <c r="C51" s="16"/>
       <c r="D51" s="3"/>
       <c r="E51" s="4"/>
       <c r="F51" s="3"/>
       <c r="G51" s="5"/>
     </row>
     <row r="52" s="1" customFormat="1" spans="3:7">
-      <c r="C52" s="17"/>
+      <c r="C52" s="16"/>
       <c r="D52" s="3"/>
       <c r="E52" s="4"/>
       <c r="F52" s="3"/>
       <c r="G52" s="5"/>
     </row>
     <row r="53" s="1" customFormat="1" spans="3:7">
-      <c r="C53" s="17"/>
+      <c r="C53" s="16"/>
       <c r="D53" s="3"/>
       <c r="E53" s="4"/>
       <c r="F53" s="3"/>
       <c r="G53" s="5"/>
     </row>
     <row r="54" s="1" customFormat="1" spans="3:7">
-      <c r="C54" s="17"/>
+      <c r="C54" s="16"/>
       <c r="D54" s="3"/>
       <c r="E54" s="4"/>
       <c r="F54" s="3"/>
       <c r="G54" s="5"/>
     </row>
     <row r="55" s="1" customFormat="1" spans="3:7">
-      <c r="C55" s="17"/>
+      <c r="C55" s="16"/>
       <c r="D55" s="3"/>
       <c r="E55" s="4"/>
       <c r="F55" s="3"/>
       <c r="G55" s="5"/>
     </row>
     <row r="56" s="1" customFormat="1" spans="3:7">
-      <c r="C56" s="17"/>
+      <c r="C56" s="16"/>
       <c r="D56" s="3"/>
       <c r="E56" s="4"/>
       <c r="F56" s="3"/>
       <c r="G56" s="5"/>
     </row>
     <row r="57" s="1" customFormat="1" spans="3:7">
-      <c r="C57" s="17"/>
+      <c r="C57" s="16"/>
       <c r="D57" s="3"/>
       <c r="E57" s="4"/>
       <c r="F57" s="3"/>
       <c r="G57" s="5"/>
     </row>
     <row r="58" s="1" customFormat="1" spans="3:7">
-      <c r="C58" s="17"/>
+      <c r="C58" s="16"/>
       <c r="D58" s="3"/>
       <c r="E58" s="4"/>
       <c r="F58" s="3"/>
       <c r="G58" s="5"/>
     </row>
     <row r="59" s="1" customFormat="1" spans="3:7">
-      <c r="C59" s="17"/>
+      <c r="C59" s="16"/>
       <c r="D59" s="3"/>
       <c r="E59" s="4"/>
       <c r="F59" s="3"/>
       <c r="G59" s="5"/>
     </row>
     <row r="60" s="1" customFormat="1" spans="3:7">
-      <c r="C60" s="17"/>
+      <c r="C60" s="16"/>
       <c r="D60" s="3"/>
       <c r="E60" s="4"/>
       <c r="F60" s="3"/>
       <c r="G60" s="5"/>
     </row>
     <row r="61" s="1" customFormat="1" spans="3:7">
-      <c r="C61" s="17"/>
+      <c r="C61" s="16"/>
       <c r="D61" s="3"/>
       <c r="E61" s="4"/>
       <c r="F61" s="3"/>
       <c r="G61" s="5"/>
     </row>
     <row r="62" s="1" customFormat="1" spans="3:7">
-      <c r="C62" s="17"/>
+      <c r="C62" s="16"/>
       <c r="D62" s="3"/>
       <c r="E62" s="4"/>
       <c r="F62" s="3"/>
       <c r="G62" s="5"/>
     </row>
     <row r="63" s="1" customFormat="1" spans="3:7">
-      <c r="C63" s="17"/>
+      <c r="C63" s="16"/>
       <c r="D63" s="3"/>
       <c r="E63" s="4"/>
       <c r="F63" s="3"/>
       <c r="G63" s="5"/>
     </row>
     <row r="64" s="1" customFormat="1" spans="3:7">
-      <c r="C64" s="17"/>
+      <c r="C64" s="16"/>
       <c r="D64" s="3"/>
       <c r="E64" s="4"/>
       <c r="F64" s="3"/>
       <c r="G64" s="5"/>
     </row>
     <row r="65" s="1" customFormat="1" spans="3:7">
-      <c r="C65" s="17"/>
+      <c r="C65" s="16"/>
       <c r="D65" s="3"/>
       <c r="E65" s="4"/>
       <c r="F65" s="3"/>
       <c r="G65" s="5"/>
     </row>
     <row r="66" s="1" customFormat="1" spans="3:7">
-      <c r="C66" s="17"/>
+      <c r="C66" s="16"/>
       <c r="D66" s="3"/>
       <c r="E66" s="4"/>
       <c r="F66" s="3"/>
       <c r="G66" s="5"/>
     </row>
     <row r="67" s="1" customFormat="1" spans="3:7">
-      <c r="C67" s="17"/>
+      <c r="C67" s="16"/>
       <c r="D67" s="3"/>
       <c r="E67" s="4"/>
       <c r="F67" s="3"/>
       <c r="G67" s="5"/>
     </row>
     <row r="68" s="1" customFormat="1" spans="3:7">
-      <c r="C68" s="17"/>
+      <c r="C68" s="16"/>
       <c r="D68" s="3"/>
       <c r="E68" s="4"/>
       <c r="F68" s="3"/>
       <c r="G68" s="5"/>
     </row>
     <row r="69" s="1" customFormat="1" spans="3:7">
-      <c r="C69" s="17"/>
+      <c r="C69" s="16"/>
       <c r="D69" s="3"/>
       <c r="E69" s="4"/>
       <c r="F69" s="3"/>
       <c r="G69" s="5"/>
     </row>
     <row r="70" s="1" customFormat="1" spans="3:7">
-      <c r="C70" s="17"/>
+      <c r="C70" s="16"/>
       <c r="D70" s="3"/>
       <c r="E70" s="4"/>
       <c r="F70" s="3"/>
       <c r="G70" s="5"/>
     </row>
     <row r="71" s="1" customFormat="1" spans="3:7">
-      <c r="C71" s="17"/>
+      <c r="C71" s="16"/>
       <c r="D71" s="3"/>
       <c r="E71" s="4"/>
       <c r="F71" s="3"/>
       <c r="G71" s="5"/>
     </row>
     <row r="72" s="1" customFormat="1" spans="3:7">
-      <c r="C72" s="17"/>
+      <c r="C72" s="16"/>
       <c r="D72" s="3"/>
       <c r="E72" s="4"/>
       <c r="F72" s="3"/>
       <c r="G72" s="5"/>
     </row>
     <row r="73" s="1" customFormat="1" spans="3:7">
-      <c r="C73" s="17"/>
+      <c r="C73" s="16"/>
       <c r="D73" s="3"/>
       <c r="E73" s="4"/>
       <c r="F73" s="3"/>
       <c r="G73" s="5"/>
     </row>
     <row r="74" s="1" customFormat="1" spans="3:7">
-      <c r="C74" s="17"/>
+      <c r="C74" s="16"/>
       <c r="D74" s="3"/>
       <c r="E74" s="4"/>
       <c r="F74" s="3"/>
       <c r="G74" s="5"/>
     </row>
     <row r="75" s="1" customFormat="1" spans="3:7">
-      <c r="C75" s="17"/>
+      <c r="C75" s="16"/>
       <c r="D75" s="3"/>
       <c r="E75" s="4"/>
       <c r="F75" s="3"/>
       <c r="G75" s="5"/>
     </row>
     <row r="76" s="1" customFormat="1" spans="3:7">
-      <c r="C76" s="17"/>
+      <c r="C76" s="16"/>
       <c r="D76" s="3"/>
       <c r="E76" s="4"/>
       <c r="F76" s="3"/>
       <c r="G76" s="5"/>
     </row>
     <row r="77" s="1" customFormat="1" spans="3:7">
-      <c r="C77" s="17"/>
+      <c r="C77" s="16"/>
       <c r="D77" s="3"/>
       <c r="E77" s="4"/>
       <c r="F77" s="3"/>
       <c r="G77" s="5"/>
     </row>
     <row r="78" s="1" customFormat="1" spans="3:7">
-      <c r="C78" s="17"/>
+      <c r="C78" s="16"/>
       <c r="D78" s="3"/>
       <c r="E78" s="4"/>
       <c r="F78" s="3"/>
       <c r="G78" s="5"/>
     </row>
     <row r="79" s="1" customFormat="1" spans="3:7">
-      <c r="C79" s="17"/>
+      <c r="C79" s="16"/>
       <c r="D79" s="3"/>
       <c r="E79" s="4"/>
       <c r="F79" s="3"/>
       <c r="G79" s="5"/>
     </row>
     <row r="80" s="1" customFormat="1" spans="3:7">
-      <c r="C80" s="17"/>
+      <c r="C80" s="16"/>
       <c r="D80" s="3"/>
       <c r="E80" s="4"/>
       <c r="F80" s="3"/>
       <c r="G80" s="5"/>
     </row>
     <row r="81" s="1" customFormat="1" spans="3:7">
-      <c r="C81" s="17"/>
+      <c r="C81" s="16"/>
       <c r="D81" s="3"/>
       <c r="E81" s="4"/>
       <c r="F81" s="3"/>
       <c r="G81" s="5"/>
     </row>
     <row r="82" s="1" customFormat="1" spans="3:7">
-      <c r="C82" s="17"/>
+      <c r="C82" s="16"/>
       <c r="D82" s="3"/>
       <c r="E82" s="4"/>
       <c r="F82" s="3"/>
       <c r="G82" s="5"/>
     </row>
     <row r="83" s="1" customFormat="1" spans="3:7">
-      <c r="C83" s="17"/>
+      <c r="C83" s="16"/>
       <c r="D83" s="3"/>
       <c r="E83" s="4"/>
       <c r="F83" s="3"/>
       <c r="G83" s="5"/>
     </row>
     <row r="84" s="1" customFormat="1" spans="3:7">
-      <c r="C84" s="17"/>
+      <c r="C84" s="16"/>
       <c r="D84" s="3"/>
       <c r="E84" s="4"/>
       <c r="F84" s="3"/>
       <c r="G84" s="5"/>
     </row>
     <row r="85" s="1" customFormat="1" spans="3:7">
-      <c r="C85" s="17"/>
+      <c r="C85" s="16"/>
       <c r="D85" s="3"/>
       <c r="E85" s="4"/>
       <c r="F85" s="3"/>
       <c r="G85" s="5"/>
     </row>
     <row r="86" s="1" customFormat="1" spans="3:7">
-      <c r="C86" s="17"/>
+      <c r="C86" s="16"/>
       <c r="D86" s="3"/>
       <c r="E86" s="4"/>
       <c r="F86" s="3"/>
       <c r="G86" s="5"/>
     </row>
     <row r="87" s="1" customFormat="1" spans="3:7">
-      <c r="C87" s="17"/>
+      <c r="C87" s="16"/>
       <c r="D87" s="3"/>
       <c r="E87" s="4"/>
       <c r="F87" s="3"/>
       <c r="G87" s="5"/>
     </row>
     <row r="88" s="1" customFormat="1" spans="3:7">
-      <c r="C88" s="17"/>
+      <c r="C88" s="16"/>
       <c r="D88" s="3"/>
       <c r="E88" s="4"/>
       <c r="F88" s="3"/>
       <c r="G88" s="5"/>
     </row>
     <row r="89" s="1" customFormat="1" spans="3:7">
-      <c r="C89" s="17"/>
+      <c r="C89" s="16"/>
       <c r="D89" s="3"/>
       <c r="E89" s="4"/>
       <c r="F89" s="3"/>
       <c r="G89" s="5"/>
     </row>
     <row r="90" s="1" customFormat="1" spans="3:7">
-      <c r="C90" s="17"/>
+      <c r="C90" s="16"/>
       <c r="D90" s="3"/>
       <c r="E90" s="4"/>
       <c r="F90" s="3"/>
       <c r="G90" s="5"/>
     </row>
     <row r="91" s="1" customFormat="1" spans="3:7">
-      <c r="C91" s="17"/>
+      <c r="C91" s="16"/>
       <c r="D91" s="3"/>
       <c r="E91" s="4"/>
       <c r="F91" s="3"/>
       <c r="G91" s="5"/>
     </row>
     <row r="92" s="1" customFormat="1" spans="3:7">
-      <c r="C92" s="17"/>
+      <c r="C92" s="16"/>
       <c r="D92" s="3"/>
       <c r="E92" s="4"/>
       <c r="F92" s="3"/>
       <c r="G92" s="5"/>
     </row>
     <row r="93" s="1" customFormat="1" spans="3:7">
-      <c r="C93" s="17"/>
+      <c r="C93" s="16"/>
       <c r="D93" s="3"/>
       <c r="E93" s="4"/>
       <c r="F93" s="3"/>
       <c r="G93" s="5"/>
     </row>
     <row r="94" s="1" customFormat="1" spans="3:7">
-      <c r="C94" s="17"/>
+      <c r="C94" s="16"/>
       <c r="D94" s="3"/>
       <c r="E94" s="4"/>
       <c r="F94" s="3"/>
       <c r="G94" s="5"/>
     </row>
     <row r="95" s="1" customFormat="1" spans="3:7">
-      <c r="C95" s="17"/>
+      <c r="C95" s="16"/>
       <c r="D95" s="3"/>
       <c r="E95" s="4"/>
       <c r="F95" s="3"/>
       <c r="G95" s="5"/>
     </row>
     <row r="96" s="1" customFormat="1" spans="3:7">
-      <c r="C96" s="17"/>
+      <c r="C96" s="16"/>
       <c r="D96" s="3"/>
       <c r="E96" s="4"/>
       <c r="F96" s="3"/>
       <c r="G96" s="5"/>
     </row>
     <row r="97" s="1" customFormat="1" spans="3:7">
-      <c r="C97" s="17"/>
+      <c r="C97" s="16"/>
       <c r="D97" s="3"/>
       <c r="E97" s="4"/>
       <c r="F97" s="3"/>
       <c r="G97" s="5"/>
     </row>
     <row r="98" s="1" customFormat="1" spans="3:7">
-      <c r="C98" s="17"/>
+      <c r="C98" s="16"/>
       <c r="D98" s="3"/>
       <c r="E98" s="4"/>
       <c r="F98" s="3"/>
       <c r="G98" s="5"/>
     </row>
     <row r="99" s="1" customFormat="1" spans="3:7">
-      <c r="C99" s="17"/>
+      <c r="C99" s="16"/>
       <c r="D99" s="3"/>
       <c r="E99" s="4"/>
       <c r="F99" s="3"/>

</xml_diff>